<commit_message>
very basic turn-taking that should be good enough for the seminar demo
</commit_message>
<xml_diff>
--- a/Last Call/Assets/Data/thoughts.xlsx
+++ b/Last Call/Assets/Data/thoughts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Topic</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>Those bastards.</t>
+  </si>
+  <si>
+    <t>Turn</t>
+  </si>
+  <si>
+    <t>Interrupt</t>
+  </si>
+  <si>
+    <t>Affinity</t>
   </si>
 </sst>
 </file>
@@ -948,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,10 +969,11 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" customWidth="1"/>
     <col min="5" max="5" width="68.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="6" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -980,43 +990,52 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1027,27 +1046,27 @@
         <v>19</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -1055,35 +1074,35 @@
         <v>19</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D5">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="D6">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>30</v>
       </c>
@@ -1091,16 +1110,16 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>31</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>32</v>
       </c>
@@ -1108,27 +1127,27 @@
         <v>19</v>
       </c>
       <c r="D8">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="Q8">
+      <c r="T8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>20</v>
       </c>
       <c r="D9">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>35</v>
       </c>
@@ -1136,49 +1155,49 @@
         <v>19</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>27</v>
       </c>
-      <c r="L10">
+      <c r="O10">
         <v>1</v>
       </c>
-      <c r="M10">
+      <c r="P10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D11">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="L11">
+      <c r="O11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D12">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c r="Q12">
+      <c r="T12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>20</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
More complex turn-taking, emotions, and argumentation.
</commit_message>
<xml_diff>
--- a/Last Call/Assets/Data/thoughts.xlsx
+++ b/Last Call/Assets/Data/thoughts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>Topic</t>
   </si>
@@ -39,118 +39,136 @@
     <t>Tangents (;)</t>
   </si>
   <si>
+    <t>Call</t>
+  </si>
+  <si>
+    <t>Orientation</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>I just got a call from command.</t>
+  </si>
+  <si>
+    <t>Complication</t>
+  </si>
+  <si>
+    <t>More malfunctions?</t>
+  </si>
+  <si>
+    <t>Defcon</t>
+  </si>
+  <si>
+    <t>Malfunction</t>
+  </si>
+  <si>
+    <t>DEFCON 1.</t>
+  </si>
+  <si>
+    <t>War</t>
+  </si>
+  <si>
+    <t>The Ruskies finally did it.</t>
+  </si>
+  <si>
+    <t>Are you sure?</t>
+  </si>
+  <si>
+    <t>Climax</t>
+  </si>
+  <si>
+    <t>We have 30 minutes to launch.</t>
+  </si>
+  <si>
+    <t>Denouement</t>
+  </si>
+  <si>
+    <t>I can't believe it.</t>
+  </si>
+  <si>
+    <t>We have no choice.</t>
+  </si>
+  <si>
+    <t>Coda</t>
+  </si>
+  <si>
+    <t>Those bastards!</t>
+  </si>
+  <si>
+    <t>About time they made the call.</t>
+  </si>
+  <si>
+    <t>And now, a shooting war.</t>
+  </si>
+  <si>
+    <t>Launch</t>
+  </si>
+  <si>
+    <t>Those bastards.</t>
+  </si>
+  <si>
+    <t>Turn</t>
+  </si>
+  <si>
+    <t>Interrupt</t>
+  </si>
+  <si>
+    <t>Affinity</t>
+  </si>
+  <si>
+    <t>Anger</t>
+  </si>
+  <si>
+    <t>Fear</t>
+  </si>
+  <si>
+    <t>Fatalism</t>
+  </si>
+  <si>
+    <t>Tribalism</t>
+  </si>
+  <si>
+    <t>Pacifism</t>
+  </si>
+  <si>
+    <t>Futurism</t>
+  </si>
+  <si>
+    <t>Ego</t>
+  </si>
+  <si>
+    <t>Respect</t>
+  </si>
+  <si>
+    <t>Militarism</t>
+  </si>
+  <si>
+    <t>Utilitarianism</t>
+  </si>
+  <si>
+    <t>Authoritarianism</t>
+  </si>
+  <si>
+    <t>Idealism</t>
+  </si>
+  <si>
+    <t>Want</t>
+  </si>
+  <si>
+    <t>Altruism</t>
+  </si>
+  <si>
     <t>Event</t>
   </si>
   <si>
-    <t>Social</t>
-  </si>
-  <si>
-    <t>Will</t>
-  </si>
-  <si>
-    <t>Love</t>
-  </si>
-  <si>
-    <t>Shame</t>
-  </si>
-  <si>
-    <t>Praise</t>
-  </si>
-  <si>
-    <t>Scare</t>
-  </si>
-  <si>
-    <t>Encourage</t>
-  </si>
-  <si>
-    <t>Mistrust</t>
-  </si>
-  <si>
-    <t>Trust</t>
-  </si>
-  <si>
-    <t>Silence</t>
-  </si>
-  <si>
-    <t>Call</t>
-  </si>
-  <si>
-    <t>Orientation</t>
-  </si>
-  <si>
-    <t>Joe</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>I just got a call from command.</t>
-  </si>
-  <si>
-    <t>Complication</t>
-  </si>
-  <si>
-    <t>More malfunctions?</t>
-  </si>
-  <si>
-    <t>Defcon</t>
-  </si>
-  <si>
-    <t>Malfunction</t>
-  </si>
-  <si>
-    <t>DEFCON 1.</t>
-  </si>
-  <si>
-    <t>War</t>
-  </si>
-  <si>
-    <t>The Ruskies finally did it.</t>
-  </si>
-  <si>
-    <t>Are you sure?</t>
-  </si>
-  <si>
-    <t>Climax</t>
-  </si>
-  <si>
-    <t>We have 30 minutes to launch.</t>
-  </si>
-  <si>
-    <t>Denouement</t>
-  </si>
-  <si>
-    <t>I can't believe it.</t>
-  </si>
-  <si>
-    <t>We have no choice.</t>
-  </si>
-  <si>
-    <t>Coda</t>
-  </si>
-  <si>
-    <t>Those bastards!</t>
-  </si>
-  <si>
-    <t>About time they made the call.</t>
-  </si>
-  <si>
-    <t>And now, a shooting war.</t>
-  </si>
-  <si>
-    <t>Launch</t>
-  </si>
-  <si>
-    <t>Those bastards.</t>
-  </si>
-  <si>
-    <t>Turn</t>
-  </si>
-  <si>
-    <t>Interrupt</t>
-  </si>
-  <si>
-    <t>Affinity</t>
+    <t>Give</t>
+  </si>
+  <si>
+    <t>Supperiority</t>
   </si>
 </sst>
 </file>
@@ -293,7 +311,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,8 +491,68 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -589,6 +667,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -634,8 +732,29 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -683,6 +802,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF9999"/>
+      <color rgb="FFCC99FF"/>
+      <color rgb="FFFFCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -957,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,12 +1095,24 @@
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" customWidth="1"/>
-    <col min="5" max="5" width="68.28515625" customWidth="1"/>
-    <col min="6" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" customWidth="1"/>
+    <col min="6" max="8" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="6" customWidth="1"/>
+    <col min="11" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="9.140625" style="11"/>
+    <col min="16" max="16" width="9.140625" style="12"/>
+    <col min="17" max="17" width="9.140625" style="13"/>
+    <col min="18" max="18" width="9.140625" style="14"/>
+    <col min="19" max="19" width="9.140625" style="15"/>
+    <col min="20" max="20" width="9.140625" style="16"/>
+    <col min="21" max="21" width="9.140625" style="17"/>
+    <col min="22" max="22" width="9.140625" style="18"/>
+    <col min="23" max="23" width="9.140625" style="19"/>
+    <col min="24" max="24" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -990,220 +1129,254 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
       </c>
       <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X1" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>17</v>
+      </c>
+      <c r="T5" s="16">
+        <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T8">
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="R8" s="14">
+        <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>22</v>
+      </c>
+      <c r="O9" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="P9" s="12">
+        <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="I10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="O10" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="P10" s="12">
+        <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="O11">
-        <v>2</v>
+        <v>29</v>
+      </c>
+      <c r="O11" s="11">
+        <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
-      </c>
-      <c r="T12">
-        <v>3</v>
+        <v>26</v>
+      </c>
+      <c r="U12" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="V12" s="18">
+        <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="O13" s="11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>